<commit_message>
Fix regressions, now makes quadratic ones
</commit_message>
<xml_diff>
--- a/Fluid Mechanics/00 data/Lab1.xlsx
+++ b/Fluid Mechanics/00 data/Lab1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Práctica 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -804,11 +804,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="20354444"/>
-        <c:axId val="17703747"/>
+        <c:axId val="5168244"/>
+        <c:axId val="98757540"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20354444"/>
+        <c:axId val="5168244"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,7 +841,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17703747"/>
+        <c:crossAx val="98757540"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -849,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17703747"/>
+        <c:axId val="98757540"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +892,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20354444"/>
+        <c:crossAx val="5168244"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1143,11 +1143,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="70774932"/>
-        <c:axId val="3125388"/>
+        <c:axId val="99652435"/>
+        <c:axId val="17342631"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70774932"/>
+        <c:axId val="99652435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1180,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3125388"/>
+        <c:crossAx val="17342631"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1188,7 +1188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3125388"/>
+        <c:axId val="17342631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70774932"/>
+        <c:crossAx val="99652435"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1295,9 +1295,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>957960</xdr:colOff>
+      <xdr:colOff>957600</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1305,8 +1305,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5429160" y="3712680"/>
-        <a:ext cx="5720400" cy="3533040"/>
+        <a:off x="5435640" y="3712680"/>
+        <a:ext cx="5726520" cy="3533040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1325,9 +1325,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>957960</xdr:colOff>
+      <xdr:colOff>957600</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1335,8 +1335,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5429160" y="7265880"/>
-        <a:ext cx="5720400" cy="3533040"/>
+        <a:off x="5435640" y="7266240"/>
+        <a:ext cx="5726520" cy="3532680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1356,11 +1356,11 @@
   </sheetPr>
   <dimension ref="B2:U31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P5" activeCellId="0" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.56"/>
   </cols>
@@ -2599,11 +2599,11 @@
   </sheetPr>
   <dimension ref="B2:J38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
@@ -2841,7 +2841,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5" t="n">
         <f aca="false">(D4*9.81)/1000</f>
         <v>0</v>
@@ -2854,20 +2854,20 @@
         <f aca="false">ROUND((1/4)*(PI()*(8/1000)^2),10)</f>
         <v>5.02655E-005</v>
       </c>
-      <c r="E12" s="4" t="e">
-        <f aca="false">1000*pow(C12, 2)/$D$12*(1-COS(PI()/2))</f>
-        <v>#NAME?</v>
+      <c r="E12" s="4" t="n">
+        <f aca="false">1000*(C12^2)/$D$12*(1-COS(PI()/2))</f>
+        <v>1.01099013560004</v>
       </c>
       <c r="F12" s="13" t="e">
         <f aca="false">100*((E12-B12)/B12)</f>
-        <v>#NAME?</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="n">
         <f aca="false">(D5*9.81)/1000</f>
         <v>0.2943</v>
@@ -2877,20 +2877,20 @@
         <v>0.000278396436525612</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="4" t="e">
-        <f aca="false">1000*pow(C13, 2)/$D$12*(1-COS(PI()/2))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F13" s="13" t="e">
+      <c r="E13" s="4" t="n">
+        <f aca="false">1000*(C13^2)/$D$12*(1-COS(PI()/2))</f>
+        <v>1.54190400712535</v>
+      </c>
+      <c r="F13" s="13" t="n">
         <f aca="false">100*((E13-B13)/B13)</f>
-        <v>#NAME?</v>
+        <v>423.922530453737</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="n">
         <f aca="false">(D6*9.81)/1000</f>
         <v>0.981</v>
@@ -2900,20 +2900,20 @@
         <v>0.00038109756097561</v>
       </c>
       <c r="D14" s="22"/>
-      <c r="E14" s="4" t="e">
-        <f aca="false">1000*pow(C14, 2)/$D$12*(1-COS(PI()/2))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F14" s="13" t="e">
+      <c r="E14" s="4" t="n">
+        <f aca="false">1000*(C14^2)/$D$12*(1-COS(PI()/2))</f>
+        <v>2.88936449416715</v>
+      </c>
+      <c r="F14" s="13" t="n">
         <f aca="false">100*((E14-B14)/B14)</f>
-        <v>#NAME?</v>
+        <v>194.532568212757</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="n">
         <f aca="false">(D7*9.81)/1000</f>
         <v>1.4715</v>
@@ -2923,20 +2923,20 @@
         <v>0.000419463087248322</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="4" t="e">
-        <f aca="false">1000*pow(C15, 2)/$D$12*(1-COS(PI()/2))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F15" s="13" t="e">
+      <c r="E15" s="4" t="n">
+        <f aca="false">1000*(C15^2)/$D$12*(1-COS(PI()/2))</f>
+        <v>3.50039851516236</v>
+      </c>
+      <c r="F15" s="13" t="n">
         <f aca="false">100*((E15-B15)/B15)</f>
-        <v>#NAME?</v>
+        <v>137.879613670564</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5" t="n">
         <f aca="false">(D8*9.81)/1000</f>
         <v>1.962</v>
@@ -2946,13 +2946,13 @@
         <v>0.000433651344319167</v>
       </c>
       <c r="D16" s="22"/>
-      <c r="E16" s="4" t="e">
-        <f aca="false">1000*pow(C16, 2)/$D$12*(1-COS(PI()/2))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F16" s="13" t="e">
+      <c r="E16" s="4" t="n">
+        <f aca="false">1000*(C16^2)/$D$12*(1-COS(PI()/2))</f>
+        <v>3.74120397548658</v>
+      </c>
+      <c r="F16" s="13" t="n">
         <f aca="false">100*((E16-B16)/B16)</f>
-        <v>#NAME?</v>
+        <v>90.6831791787248</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -3026,7 +3026,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="n">
         <f aca="false">9.81*G4/1000</f>
         <v>0</v>
@@ -3040,8 +3040,8 @@
         <v>5.02655E-005</v>
       </c>
       <c r="E22" s="4" t="n">
-        <f aca="false">1000*((C22^2)/D22)*(1-COS((2/3)*PI()))</f>
-        <v>0.9611674094</v>
+        <f aca="false">1000*((C22^2)/$D$22)*(1-COS((2/3)*PI()))</f>
+        <v>0.961167409420643</v>
       </c>
       <c r="F22" s="13" t="e">
         <f aca="false">100*((E22-B22)/B22)</f>
@@ -3052,7 +3052,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="n">
         <f aca="false">9.81*G5/1000</f>
         <v>0.2943</v>
@@ -3063,19 +3063,19 @@
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="4" t="n">
-        <f aca="false">1000*((C23^2)/D22)*(1-COS((2/3)*PI()))</f>
-        <v>2.126599493</v>
+        <f aca="false">1000*((C23^2)/$D$22)*(1-COS((2/3)*PI()))</f>
+        <v>2.12659949328303</v>
       </c>
       <c r="F23" s="13" t="n">
         <f aca="false">100*((E23-B23)/B23)</f>
-        <v>622.595818212708</v>
+        <v>622.595818308877</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="n">
         <f aca="false">9.81*G6/1000</f>
         <v>0.981</v>
@@ -3086,19 +3086,19 @@
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="4" t="n">
-        <f aca="false">1000*((C24^2)/D22)*(1-COS((2/3)*PI()))</f>
-        <v>2.98845752</v>
+        <f aca="false">1000*((C24^2)/$D$22)*(1-COS((2/3)*PI()))</f>
+        <v>2.98845752033788</v>
       </c>
       <c r="F24" s="13" t="n">
         <f aca="false">100*((E24-B24)/B24)</f>
-        <v>204.633794087666</v>
+        <v>204.633794122108</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="5" t="n">
         <f aca="false">9.81*G7/1000</f>
         <v>1.4715</v>
@@ -3109,19 +3109,19 @@
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="4" t="n">
-        <f aca="false">1000*((C25^2)/D22)*(1-COS((2/3)*PI()))</f>
-        <v>3.471309367</v>
+        <f aca="false">1000*((C25^2)/$D$22)*(1-COS((2/3)*PI()))</f>
+        <v>3.4713093669196</v>
       </c>
       <c r="F25" s="13" t="n">
         <f aca="false">100*((E25-B25)/B25)</f>
-        <v>135.902777234115</v>
+        <v>135.902777228651</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="5" t="n">
         <f aca="false">9.81*G8/1000</f>
         <v>1.962</v>
@@ -3211,7 +3211,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="5" t="n">
         <f aca="false">9.81*J4/1000</f>
         <v>0</v>
@@ -3225,8 +3225,8 @@
         <v>5.02655E-005</v>
       </c>
       <c r="E32" s="4" t="n">
-        <f aca="false">1000*((C32^2)/$D$22)*(1-COS((2/3)*PI()))</f>
-        <v>0.777819541818253</v>
+        <f aca="false">1000*((C32^2)/$D$32)*(1-COS((PI())))</f>
+        <v>1.03709272242434</v>
       </c>
       <c r="F32" s="13" t="e">
         <f aca="false">100*((E32-B32)/B32)</f>
@@ -3237,7 +3237,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="5" t="n">
         <f aca="false">9.81*J5/1000</f>
         <v>0.2943</v>
@@ -3248,19 +3248,19 @@
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="4" t="n">
-        <f aca="false">1000*((C33^2)/$D$22)*(1-COS((2/3)*PI()))</f>
-        <v>1.23580784508135</v>
+        <f aca="false">1000*((C33^2)/$D$32)*(1-COS((PI())))</f>
+        <v>1.64774379344179</v>
       </c>
       <c r="F33" s="13" t="n">
         <f aca="false">100*((E33-B33)/B33)</f>
-        <v>319.914320448979</v>
+        <v>459.885760598636</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="5" t="n">
         <f aca="false">9.81*J6/1000</f>
         <v>0.4905</v>
@@ -3271,19 +3271,19 @@
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="4" t="n">
-        <f aca="false">1000*((C34^2)/$D$22)*(1-COS((2/3)*PI()))</f>
-        <v>1.30279434144467</v>
+        <f aca="false">1000*((C34^2)/$D$32)*(1-COS((PI())))</f>
+        <v>1.73705912192623</v>
       </c>
       <c r="F34" s="13" t="n">
         <f aca="false">100*((E34-B34)/B34)</f>
-        <v>165.60537032511</v>
+        <v>254.140493766814</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="5" t="n">
         <f aca="false">9.81*J7/1000</f>
         <v>0.981</v>
@@ -3294,19 +3294,19 @@
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="4" t="n">
-        <f aca="false">1000*((C35^2)/$D$22)*(1-COS((2/3)*PI()))</f>
-        <v>1.79443118958905</v>
+        <f aca="false">1000*((C35^2)/$D$32)*(1-COS((PI())))</f>
+        <v>2.39257491945207</v>
       </c>
       <c r="F35" s="13" t="n">
         <f aca="false">100*((E35-B35)/B35)</f>
-        <v>82.9185718235529</v>
+        <v>143.89142909807</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="5" t="n">
         <f aca="false">9.81*J8/1000</f>
         <v>1.962</v>
@@ -3317,12 +3317,12 @@
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="4" t="n">
-        <f aca="false">1000*((C36^2)/$D$22)*(1-COS((2/3)*PI()))</f>
-        <v>2.85325916534298</v>
+        <f aca="false">1000*((C36^2)/$D$32)*(1-COS((PI())))</f>
+        <v>3.80434555379065</v>
       </c>
       <c r="F36" s="13" t="n">
         <f aca="false">100*((E36-B36)/B36)</f>
-        <v>45.4260532794587</v>
+        <v>93.9014043726121</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>

</xml_diff>